<commit_message>
Updating scripts for better logging
</commit_message>
<xml_diff>
--- a/CDMO_Automation/00_Annual_Update/Reserve_Level_Template/figure_files/Reserve_Level_Plotting_Variables.xlsx
+++ b/CDMO_Automation/00_Annual_Update/Reserve_Level_Template/figure_files/Reserve_Level_Plotting_Variables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global_Decisions--&gt;" sheetId="1" state="visible" r:id="rId2"/>
@@ -524,10 +524,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="1" sqref="A12:B12 C23"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -547,10 +547,10 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="1" sqref="A12:B12 J9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -797,13 +797,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="1" sqref="A12:B12 O10"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
   </cols>
@@ -830,6 +830,11 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -851,11 +856,11 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="1" sqref="A12:B12 G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.45"/>
   </cols>
@@ -873,12 +878,12 @@
         <v>2007</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2016</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2016</v>
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -899,11 +904,11 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="1" sqref="A12:B12 G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.44"/>
@@ -1135,10 +1140,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="A12:B12 C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.19"/>
@@ -1261,11 +1266,11 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12:B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.11"/>
   </cols>
@@ -1386,10 +1391,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="1" sqref="A12:B12 G33"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1409,10 +1414,10 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="1" sqref="A12:B12 F10"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
@@ -1456,7 +1461,7 @@
         <v>59</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1821,10 +1826,10 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="1" sqref="A12:B12 N7"/>
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>

</xml_diff>